<commit_message>
Updte 8-Jul-2021, midday update.
</commit_message>
<xml_diff>
--- a/ANDREAS-KODYAT-TaxList.xlsx
+++ b/ANDREAS-KODYAT-TaxList.xlsx
@@ -3100,7 +3100,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3562,6 +3562,11 @@
     <row r="18" spans="1:11">
       <c r="F18" s="1"/>
     </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="2">
+        <v>44197</v>
+      </c>
+    </row>
     <row r="25" spans="1:11">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>

</xml_diff>

<commit_message>
Update 14-Jul-2021, end of days.
</commit_message>
<xml_diff>
--- a/ANDREAS-KODYAT-TaxList.xlsx
+++ b/ANDREAS-KODYAT-TaxList.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="DPP 2019" sheetId="1" r:id="rId1"/>
-    <sheet name="DPP 2020" sheetId="3" r:id="rId2"/>
-    <sheet name="DPP 2021" sheetId="2" r:id="rId3"/>
+    <sheet name="DPP 2018" sheetId="4" r:id="rId1"/>
+    <sheet name="DPP 2019" sheetId="1" r:id="rId2"/>
+    <sheet name="DPP 2020" sheetId="3" r:id="rId3"/>
+    <sheet name="DPP 2021" sheetId="2" r:id="rId4"/>
+    <sheet name="Summary" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="127">
   <si>
     <t>Faktur Pajak</t>
   </si>
@@ -325,6 +327,78 @@
   </si>
   <si>
     <t>TOTAL DES</t>
+  </si>
+  <si>
+    <t>010.003-18.80597508</t>
+  </si>
+  <si>
+    <t>080.003-18.80597506</t>
+  </si>
+  <si>
+    <t>080.003-18.80597668</t>
+  </si>
+  <si>
+    <t>010.003-18.80597731</t>
+  </si>
+  <si>
+    <t>010.003-18.80597730</t>
+  </si>
+  <si>
+    <t>080.003-18.80597722</t>
+  </si>
+  <si>
+    <t>080.005-18.74392958</t>
+  </si>
+  <si>
+    <t>010.005-18.74393007</t>
+  </si>
+  <si>
+    <t>010.005-18.74393171</t>
+  </si>
+  <si>
+    <t>010.005-18.74393235</t>
+  </si>
+  <si>
+    <t>080.005-18.73293465</t>
+  </si>
+  <si>
+    <t>Tahun</t>
+  </si>
+  <si>
+    <t>DPP Pembelian</t>
+  </si>
+  <si>
+    <t>PPN Pembelian</t>
+  </si>
+  <si>
+    <t>010.000-18.89294848</t>
+  </si>
+  <si>
+    <t>080.000-18.89294964</t>
+  </si>
+  <si>
+    <t>010.000-18.89294967</t>
+  </si>
+  <si>
+    <t>010.000-18.89294968</t>
+  </si>
+  <si>
+    <t>010.000-18.89295053</t>
+  </si>
+  <si>
+    <t>080.000-18.89295109</t>
+  </si>
+  <si>
+    <t>010.000-18.89295132</t>
+  </si>
+  <si>
+    <t>080.000-18.89295320</t>
+  </si>
+  <si>
+    <t>010.000-18.89295373</t>
+  </si>
+  <si>
+    <t>080.000-18.89295964</t>
   </si>
 </sst>
 </file>
@@ -409,6 +483,266 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tahun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Summary!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DPP Pembelian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Summary!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#.##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>781156821</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>685649947</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>372107729</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128712638</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PPN Pembelian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Summary!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>#.##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>78115682.100000009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41109594.70000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20639272.900000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11241263.800000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="91643904"/>
+        <c:axId val="91645440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="91643904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91645440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91645440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91643904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,11 +1030,722 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2">
+        <v>43102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="3">
+        <v>6000000</v>
+      </c>
+      <c r="H2" s="3">
+        <f>G2*0.1</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2">
+        <v>43108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="3">
+        <v>10500000</v>
+      </c>
+      <c r="H3" s="3">
+        <f>G3*0.1</f>
+        <v>1050000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2">
+        <v>43108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3">
+        <v>19090909</v>
+      </c>
+      <c r="H4" s="3">
+        <f>G4*0.1</f>
+        <v>1909090.9000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2">
+        <v>43108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="3">
+        <v>76818182</v>
+      </c>
+      <c r="H5" s="3">
+        <f>G5*0.1</f>
+        <v>7681818.2000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2">
+        <v>43110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="3">
+        <v>74545455</v>
+      </c>
+      <c r="H6" s="3">
+        <f>G6*0.1</f>
+        <v>7454545.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2">
+        <v>43113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="3">
+        <v>23350000</v>
+      </c>
+      <c r="H7" s="3">
+        <f>G7*0.1</f>
+        <v>2335000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2">
+        <v>43116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3">
+        <v>69454546</v>
+      </c>
+      <c r="H8" s="3">
+        <f>G8*0.1</f>
+        <v>6945454.6000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2">
+        <v>43123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="3">
+        <v>14000000</v>
+      </c>
+      <c r="H9" s="3">
+        <f>G9*0.1</f>
+        <v>1400000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2">
+        <v>43125</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="3">
+        <v>12654546</v>
+      </c>
+      <c r="H10" s="3">
+        <f>G10*0.1</f>
+        <v>1265454.6000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2">
+        <v>43151</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="3">
+        <v>76681818</v>
+      </c>
+      <c r="H11" s="3">
+        <f>G11*0.1</f>
+        <v>7668181.8000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2">
+        <v>43152</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="3">
+        <v>22350000</v>
+      </c>
+      <c r="H12" s="3">
+        <f>G12*0.1</f>
+        <v>2235000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2">
+        <v>43255</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2136364</v>
+      </c>
+      <c r="H13" s="3">
+        <f>G13*0.1</f>
+        <v>213636.40000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2">
+        <v>43255</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="3">
+        <v>17325000</v>
+      </c>
+      <c r="H14" s="3">
+        <f>G14*0.1</f>
+        <v>1732500</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2">
+        <v>43277</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5500000</v>
+      </c>
+      <c r="H15" s="3">
+        <f>G15*0.1</f>
+        <v>550000</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2">
+        <v>43279</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="3">
+        <v>193500000</v>
+      </c>
+      <c r="H16" s="3">
+        <f>G16*0.1</f>
+        <v>19350000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2">
+        <v>43279</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="3">
+        <v>41090909</v>
+      </c>
+      <c r="H17" s="3">
+        <f>G17*0.1</f>
+        <v>4109090.9000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="2">
+        <v>43279</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="3">
+        <v>21275000</v>
+      </c>
+      <c r="H18" s="3">
+        <f>G18*0.1</f>
+        <v>2127500</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="2">
+        <v>43428</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="3">
+        <v>22500000</v>
+      </c>
+      <c r="H19" s="3">
+        <f>G19*0.1</f>
+        <v>2250000</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2">
+        <v>43431</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="3">
+        <v>36245455</v>
+      </c>
+      <c r="H20" s="3">
+        <f>G20*0.1</f>
+        <v>3624545.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2">
+        <v>43439</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="3">
+        <v>15545455</v>
+      </c>
+      <c r="H21" s="3">
+        <f>G21*0.1</f>
+        <v>1554545.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="2">
+        <v>43444</v>
+      </c>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="3">
+        <v>9818182</v>
+      </c>
+      <c r="H22" s="3">
+        <f>G22*0.1</f>
+        <v>981818.20000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="2">
+        <v>43453</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="3">
+        <v>10775000</v>
+      </c>
+      <c r="H23" s="3">
+        <f>G23*0.1</f>
+        <v>1077500</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="D25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="D26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="21">
+        <f>SUM(G2:G29)</f>
+        <v>781156821</v>
+      </c>
+      <c r="H30" s="21">
+        <f>SUM(H2:H29)</f>
+        <v>78115682.100000009</v>
+      </c>
+      <c r="I30" s="6"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:I23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2045,84 +3090,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="8" t="s">
+    <row r="56" spans="1:11">
+      <c r="A56" s="5"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G55" s="9">
-        <f>SUM(G2:G54)</f>
+      <c r="G56" s="9">
+        <f>SUM(G2:G55)</f>
         <v>685649947</v>
       </c>
-      <c r="H55" s="9">
-        <f>SUM(H2:H54)</f>
+      <c r="H56" s="9">
+        <f>SUM(H2:H55)</f>
         <v>41109594.70000001</v>
       </c>
-      <c r="I55" s="6"/>
-      <c r="J55" s="9">
-        <f t="shared" ref="J55:K55" si="1">SUM(J2:J54)</f>
+      <c r="I56" s="6"/>
+      <c r="J56" s="9">
+        <f t="shared" ref="J56:K56" si="1">SUM(J2:J55)</f>
         <v>685649947</v>
       </c>
-      <c r="K55" s="9">
+      <c r="K56" s="9">
         <f t="shared" si="1"/>
         <v>41109594.700000003</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1">
-      <c r="A56" s="10"/>
-      <c r="F56" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G56" s="13">
-        <f>G58-G55</f>
-        <v>3763860</v>
-      </c>
-      <c r="H56" s="13"/>
-      <c r="J56" s="14" t="str">
-        <f>IF(G55=J55,"Ok!","Re check!")</f>
-        <v>Ok!</v>
-      </c>
-      <c r="K56" s="14" t="str">
-        <f>IF(H55=K55,"Ok!","Re check!")</f>
-        <v>Ok!</v>
-      </c>
-    </row>
     <row r="57" spans="1:11" s="11" customFormat="1">
       <c r="A57" s="10"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="13"/>
+      <c r="F57" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G57" s="13">
+        <f>G59-G56</f>
+        <v>3763860</v>
+      </c>
       <c r="H57" s="13"/>
-      <c r="J57" s="14"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="E58" s="15" t="s">
+      <c r="J57" s="14" t="str">
+        <f>IF(G56=J56,"Ok!","Re check!")</f>
+        <v>Ok!</v>
+      </c>
+      <c r="K57" s="14" t="str">
+        <f>IF(H56=K56,"Ok!","Re check!")</f>
+        <v>Ok!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="11" customFormat="1">
+      <c r="A58" s="10"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="E59" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F59" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G58" s="16">
+      <c r="G59" s="16">
         <v>689413807</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="F59" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G59" s="16">
-        <v>4927888</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="F60" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G60" s="16">
+        <v>4927888</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="F61" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G60" s="9">
-        <f>SUM(G58:G59)</f>
+      <c r="G61" s="9">
+        <f>SUM(G59:G60)</f>
         <v>694341695</v>
       </c>
     </row>
@@ -2135,13 +3180,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2210,8 +3255,7 @@
         <v>12000000</v>
       </c>
       <c r="H2" s="3">
-        <f>G2*0.1</f>
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
@@ -2240,8 +3284,7 @@
         <v>34350000</v>
       </c>
       <c r="H3" s="3">
-        <f>G3*0.1</f>
-        <v>3435000</v>
+        <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
@@ -2292,7 +3335,7 @@
       </c>
       <c r="K5" s="19">
         <f>SUM(H2:H4)</f>
-        <v>4940454.5999999996</v>
+        <v>305454.60000000003</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2318,8 +3361,7 @@
         <v>5500000</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>550000</v>
+        <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
@@ -2375,8 +3417,7 @@
         <v>11750000</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>1175000</v>
+        <v>0</v>
       </c>
       <c r="I8" t="s">
         <v>16</v>
@@ -2400,7 +3441,7 @@
       </c>
       <c r="K9" s="19">
         <f>SUM(H6:H8)</f>
-        <v>1915909.1</v>
+        <v>190909.1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2504,8 +3545,7 @@
         <v>2765000</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>276500</v>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
         <v>16</v>
@@ -2561,8 +3601,7 @@
         <v>5500000</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>550000</v>
+        <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>16</v>
@@ -2613,7 +3652,7 @@
       </c>
       <c r="K17" s="19">
         <f>SUM(H12:H16)</f>
-        <v>2144681.9</v>
+        <v>1318181.8999999999</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2639,8 +3678,7 @@
         <v>10550000</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="0"/>
-        <v>1055000</v>
+        <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>
@@ -2669,8 +3707,7 @@
         <v>31000000</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>3100000</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>16</v>
@@ -2694,7 +3731,7 @@
       </c>
       <c r="K20" s="19">
         <f>SUM(H18:H19)</f>
-        <v>4155000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2720,8 +3757,7 @@
         <v>5250000</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="0"/>
-        <v>525000</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
@@ -2745,7 +3781,7 @@
       </c>
       <c r="K22" s="19">
         <f>H21</f>
-        <v>525000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2771,8 +3807,7 @@
         <v>5500000</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="0"/>
-        <v>550000</v>
+        <v>0</v>
       </c>
       <c r="I23" t="s">
         <v>16</v>
@@ -2796,7 +3831,7 @@
       </c>
       <c r="K24" s="19">
         <f>H23</f>
-        <v>550000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2822,8 +3857,7 @@
         <v>10550000</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="0"/>
-        <v>1055000</v>
+        <v>0</v>
       </c>
       <c r="I25" t="s">
         <v>16</v>
@@ -2874,7 +3908,7 @@
       </c>
       <c r="K27" s="19">
         <f>SUM(H25:H26)</f>
-        <v>1203636.3999999999</v>
+        <v>148636.4</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2951,8 +3985,7 @@
         <v>5500000</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="0"/>
-        <v>550000</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
         <v>16</v>
@@ -3008,8 +4041,7 @@
         <v>25500000</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="0"/>
-        <v>2550000</v>
+        <v>0</v>
       </c>
       <c r="I32" t="s">
         <v>16</v>
@@ -3033,7 +4065,7 @@
       </c>
       <c r="K33" s="19">
         <f>SUM(H30:H32)</f>
-        <v>15536090.9</v>
+        <v>12436090.9</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -3060,7 +4092,7 @@
       </c>
       <c r="H38" s="21">
         <f>SUM(H2:H37)</f>
-        <v>37210772.899999999</v>
+        <v>20639272.900000002</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="21">
@@ -3069,7 +4101,7 @@
       </c>
       <c r="K38" s="21">
         <f t="shared" si="1"/>
-        <v>37210772.899999999</v>
+        <v>20639272.899999999</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -3094,13 +4126,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3562,11 +4594,6 @@
     <row r="18" spans="1:11">
       <c r="F18" s="1"/>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="2">
-        <v>44197</v>
-      </c>
-    </row>
     <row r="25" spans="1:11">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
@@ -3622,4 +4649,88 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="4">
+        <f>'DPP 2018'!G30</f>
+        <v>781156821</v>
+      </c>
+      <c r="C2" s="4">
+        <f>'DPP 2018'!H30</f>
+        <v>78115682.100000009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="4">
+        <f>'DPP 2019'!G56</f>
+        <v>685649947</v>
+      </c>
+      <c r="C3" s="4">
+        <f>'DPP 2019'!H56</f>
+        <v>41109594.70000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="4">
+        <f>'DPP 2020'!G38</f>
+        <v>372107729</v>
+      </c>
+      <c r="C4" s="4">
+        <f>'DPP 2020'!H38</f>
+        <v>20639272.900000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="4">
+        <f>'DPP 2021'!G25</f>
+        <v>128712638</v>
+      </c>
+      <c r="C5" s="4">
+        <f>'DPP 2021'!H25</f>
+        <v>11241263.800000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 15-Jul-2021, end of day update.
</commit_message>
<xml_diff>
--- a/ANDREAS-KODYAT-TaxList.xlsx
+++ b/ANDREAS-KODYAT-TaxList.xlsx
@@ -4,21 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DPP 2018" sheetId="4" r:id="rId1"/>
-    <sheet name="DPP 2019" sheetId="1" r:id="rId2"/>
-    <sheet name="DPP 2020" sheetId="3" r:id="rId3"/>
-    <sheet name="DPP 2021" sheetId="2" r:id="rId4"/>
-    <sheet name="Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="Sales 2019" sheetId="6" r:id="rId2"/>
+    <sheet name="DPP 2019" sheetId="1" r:id="rId3"/>
+    <sheet name="Sales 2020" sheetId="7" r:id="rId4"/>
+    <sheet name="DPP 2020" sheetId="3" r:id="rId5"/>
+    <sheet name="Sales 2021" sheetId="8" r:id="rId6"/>
+    <sheet name="DPP 2021" sheetId="2" r:id="rId7"/>
+    <sheet name="Summary" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="146">
   <si>
     <t>Faktur Pajak</t>
   </si>
@@ -399,6 +402,63 @@
   </si>
   <si>
     <t>080.000-18.89295964</t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Mei</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Agt</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Okt</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Des</t>
+  </si>
+  <si>
+    <t>DPP BELI 2019</t>
+  </si>
+  <si>
+    <t>Est -sales</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>Setoran PPH</t>
   </si>
 </sst>
 </file>
@@ -452,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -476,6 +536,7 @@
     <xf numFmtId="17" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,7 +657,7 @@
                   <c:v>781156821</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>685649947</c:v>
+                  <c:v>689413807</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>372107729</c:v>
@@ -665,25 +726,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91643904"/>
-        <c:axId val="91645440"/>
+        <c:axId val="125521280"/>
+        <c:axId val="125531264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91643904"/>
+        <c:axId val="125521280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91645440"/>
+        <c:crossAx val="125531264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91645440"/>
+        <c:axId val="125531264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,20 +752,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91643904"/>
+        <c:crossAx val="125521280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1032,9 +1092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1101,7 +1161,7 @@
         <v>6000000</v>
       </c>
       <c r="H2" s="3">
-        <f>G2*0.1</f>
+        <f t="shared" ref="H2:H23" si="0">G2*0.1</f>
         <v>600000</v>
       </c>
     </row>
@@ -1128,7 +1188,7 @@
         <v>10500000</v>
       </c>
       <c r="H3" s="3">
-        <f>G3*0.1</f>
+        <f t="shared" si="0"/>
         <v>1050000</v>
       </c>
       <c r="I3" t="s">
@@ -1158,7 +1218,7 @@
         <v>19090909</v>
       </c>
       <c r="H4" s="3">
-        <f>G4*0.1</f>
+        <f t="shared" si="0"/>
         <v>1909090.9000000001</v>
       </c>
     </row>
@@ -1185,7 +1245,7 @@
         <v>76818182</v>
       </c>
       <c r="H5" s="3">
-        <f>G5*0.1</f>
+        <f t="shared" si="0"/>
         <v>7681818.2000000002</v>
       </c>
     </row>
@@ -1212,7 +1272,7 @@
         <v>74545455</v>
       </c>
       <c r="H6" s="3">
-        <f>G6*0.1</f>
+        <f t="shared" si="0"/>
         <v>7454545.5</v>
       </c>
     </row>
@@ -1239,7 +1299,7 @@
         <v>23350000</v>
       </c>
       <c r="H7" s="3">
-        <f>G7*0.1</f>
+        <f t="shared" si="0"/>
         <v>2335000</v>
       </c>
       <c r="I7" t="s">
@@ -1269,7 +1329,7 @@
         <v>69454546</v>
       </c>
       <c r="H8" s="3">
-        <f>G8*0.1</f>
+        <f t="shared" si="0"/>
         <v>6945454.6000000006</v>
       </c>
     </row>
@@ -1296,7 +1356,7 @@
         <v>14000000</v>
       </c>
       <c r="H9" s="3">
-        <f>G9*0.1</f>
+        <f t="shared" si="0"/>
         <v>1400000</v>
       </c>
       <c r="I9" t="s">
@@ -1326,7 +1386,7 @@
         <v>12654546</v>
       </c>
       <c r="H10" s="3">
-        <f>G10*0.1</f>
+        <f t="shared" si="0"/>
         <v>1265454.6000000001</v>
       </c>
     </row>
@@ -1353,7 +1413,7 @@
         <v>76681818</v>
       </c>
       <c r="H11" s="3">
-        <f>G11*0.1</f>
+        <f t="shared" si="0"/>
         <v>7668181.8000000007</v>
       </c>
     </row>
@@ -1380,7 +1440,7 @@
         <v>22350000</v>
       </c>
       <c r="H12" s="3">
-        <f>G12*0.1</f>
+        <f t="shared" si="0"/>
         <v>2235000</v>
       </c>
       <c r="I12" t="s">
@@ -1410,7 +1470,7 @@
         <v>2136364</v>
       </c>
       <c r="H13" s="3">
-        <f>G13*0.1</f>
+        <f t="shared" si="0"/>
         <v>213636.40000000002</v>
       </c>
     </row>
@@ -1437,7 +1497,7 @@
         <v>17325000</v>
       </c>
       <c r="H14" s="3">
-        <f>G14*0.1</f>
+        <f t="shared" si="0"/>
         <v>1732500</v>
       </c>
       <c r="I14" t="s">
@@ -1467,7 +1527,7 @@
         <v>5500000</v>
       </c>
       <c r="H15" s="3">
-        <f>G15*0.1</f>
+        <f t="shared" si="0"/>
         <v>550000</v>
       </c>
       <c r="I15" t="s">
@@ -1497,7 +1557,7 @@
         <v>193500000</v>
       </c>
       <c r="H16" s="3">
-        <f>G16*0.1</f>
+        <f t="shared" si="0"/>
         <v>19350000</v>
       </c>
     </row>
@@ -1524,7 +1584,7 @@
         <v>41090909</v>
       </c>
       <c r="H17" s="3">
-        <f>G17*0.1</f>
+        <f t="shared" si="0"/>
         <v>4109090.9000000004</v>
       </c>
     </row>
@@ -1551,7 +1611,7 @@
         <v>21275000</v>
       </c>
       <c r="H18" s="3">
-        <f>G18*0.1</f>
+        <f t="shared" si="0"/>
         <v>2127500</v>
       </c>
       <c r="I18" t="s">
@@ -1581,7 +1641,7 @@
         <v>22500000</v>
       </c>
       <c r="H19" s="3">
-        <f>G19*0.1</f>
+        <f t="shared" si="0"/>
         <v>2250000</v>
       </c>
       <c r="I19" t="s">
@@ -1611,7 +1671,7 @@
         <v>36245455</v>
       </c>
       <c r="H20" s="3">
-        <f>G20*0.1</f>
+        <f t="shared" si="0"/>
         <v>3624545.5</v>
       </c>
     </row>
@@ -1638,7 +1698,7 @@
         <v>15545455</v>
       </c>
       <c r="H21" s="3">
-        <f>G21*0.1</f>
+        <f t="shared" si="0"/>
         <v>1554545.5</v>
       </c>
     </row>
@@ -1665,7 +1725,7 @@
         <v>9818182</v>
       </c>
       <c r="H22" s="3">
-        <f>G22*0.1</f>
+        <f t="shared" si="0"/>
         <v>981818.20000000007</v>
       </c>
     </row>
@@ -1692,7 +1752,7 @@
         <v>10775000</v>
       </c>
       <c r="H23" s="3">
-        <f>G23*0.1</f>
+        <f t="shared" si="0"/>
         <v>1077500</v>
       </c>
       <c r="I23" t="s">
@@ -1741,11 +1801,341 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3">
+        <v>60754900</v>
+      </c>
+      <c r="C2" s="23">
+        <f>B2/$B$15</f>
+        <v>8.2988328363234234E-2</v>
+      </c>
+      <c r="D2" s="3">
+        <f>'DPP 2019'!J7</f>
+        <v>59147727</v>
+      </c>
+      <c r="F2" s="3">
+        <f>B2*0.005</f>
+        <v>303774.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="3">
+        <v>58850000</v>
+      </c>
+      <c r="C3" s="23">
+        <f t="shared" ref="C3:C13" si="0">B3/$B$15</f>
+        <v>8.0386324793166222E-2</v>
+      </c>
+      <c r="D3" s="3">
+        <f>'DPP 2019'!J10</f>
+        <v>40395455</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F13" si="1">B3*0.005</f>
+        <v>294250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="3">
+        <v>65250000</v>
+      </c>
+      <c r="C4" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9128422986475719E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <f>'DPP 2019'!J13</f>
+        <v>31250000</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>326250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="3">
+        <v>60280500</v>
+      </c>
+      <c r="C5" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2340320334655173E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>'DPP 2019'!J17</f>
+        <v>96388091</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>301402.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3">
+        <v>54750000</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" si="0"/>
+        <v>7.4785918138077334E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <f>'DPP 2019'!J22</f>
+        <v>43727273</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>273750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3">
+        <v>71450000</v>
+      </c>
+      <c r="C7" s="23">
+        <f t="shared" si="0"/>
+        <v>9.7597330611244301E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <f>'DPP 2019'!J25</f>
+        <v>55018182</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>357250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="3">
+        <v>68110000</v>
+      </c>
+      <c r="C8" s="23">
+        <f t="shared" si="0"/>
+        <v>9.3035048116610897E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <f>'DPP 2019'!J33</f>
+        <v>201112219</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>340550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="3">
+        <v>58450500</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" si="0"/>
+        <v>7.984062663250574E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f>'DPP 2019'!J37</f>
+        <v>42786000</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>292252.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="3">
+        <v>53956500</v>
+      </c>
+      <c r="C10" s="23">
+        <f t="shared" si="0"/>
+        <v>7.3702034557391216E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <f>'DPP 2019'!J41</f>
+        <v>11081818</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>269782.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="3">
+        <v>62370200</v>
+      </c>
+      <c r="C11" s="23">
+        <f t="shared" si="0"/>
+        <v>8.5194751990054995E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f>'DPP 2019'!J46</f>
+        <v>41643182</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>311851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="3">
+        <v>59367700</v>
+      </c>
+      <c r="C12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.1093478579834399E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <f>'DPP 2019'!J50</f>
+        <v>63100000</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>296838.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="3">
+        <v>58499395</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" si="0"/>
+        <v>7.9907414896749782E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <f>'DPP 2019'!J52</f>
+        <v>3763860</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>292496.97500000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3">
+        <f>SUM(B2:B13)</f>
+        <v>732089695</v>
+      </c>
+      <c r="D15" s="3">
+        <f>SUM(D2:D13)</f>
+        <v>689413807</v>
+      </c>
+      <c r="F15" s="3">
+        <f>SUM(F2:F13)</f>
+        <v>3660448.4750000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B15-B19</f>
+        <v>3030915.25</v>
+      </c>
+      <c r="F16" s="23">
+        <f>F15/B15</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="3">
+        <f>'DPP 2019'!G61</f>
+        <v>694341695</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="3">
+        <f>B18*1.05</f>
+        <v>729058779.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3090,6 +3480,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="2">
+        <v>43811</v>
+      </c>
+      <c r="G51" s="4">
+        <v>3763860</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="I52" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="J52" s="19">
+        <v>3763860</v>
+      </c>
+    </row>
     <row r="56" spans="1:11">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
@@ -3101,7 +3510,7 @@
       </c>
       <c r="G56" s="9">
         <f>SUM(G2:G55)</f>
-        <v>685649947</v>
+        <v>689413807</v>
       </c>
       <c r="H56" s="9">
         <f>SUM(H2:H55)</f>
@@ -3110,7 +3519,7 @@
       <c r="I56" s="6"/>
       <c r="J56" s="9">
         <f t="shared" ref="J56:K56" si="1">SUM(J2:J55)</f>
-        <v>685649947</v>
+        <v>689413807</v>
       </c>
       <c r="K56" s="9">
         <f t="shared" si="1"/>
@@ -3124,7 +3533,7 @@
       </c>
       <c r="G57" s="13">
         <f>G59-G56</f>
-        <v>3763860</v>
+        <v>0</v>
       </c>
       <c r="H57" s="13"/>
       <c r="J57" s="14" t="str">
@@ -3180,13 +3589,357 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42500000</v>
+      </c>
+      <c r="C2" s="23">
+        <f>B2/$B$15</f>
+        <v>0.10787233245999046</v>
+      </c>
+      <c r="D2" s="3">
+        <f>'DPP 2020'!J5</f>
+        <v>49404546</v>
+      </c>
+      <c r="F2" s="3">
+        <f>B2*0.005</f>
+        <v>212500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43445500</v>
+      </c>
+      <c r="C3" s="23">
+        <f t="shared" ref="C3:C13" si="0">B3/$B$15</f>
+        <v>0.1102721745856592</v>
+      </c>
+      <c r="D3" s="3">
+        <f>'DPP 2020'!J9</f>
+        <v>19159091</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F13" si="1">B3*0.005</f>
+        <v>217227.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="3">
+        <v>31450000</v>
+      </c>
+      <c r="C4" s="23">
+        <f t="shared" si="0"/>
+        <v>7.9825526020392945E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <f>'DPP 2020'!J11</f>
+        <v>36900000</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>157250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="3">
+        <v>36599500</v>
+      </c>
+      <c r="C5" s="23">
+        <f t="shared" si="0"/>
+        <v>9.289584545575108E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>'DPP 2020'!J17</f>
+        <v>21446819</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>182997.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3">
+        <v>25775500</v>
+      </c>
+      <c r="C6" s="23">
+        <f t="shared" si="0"/>
+        <v>6.5422666007587865E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8520000</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>128877.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3">
+        <v>29443750</v>
+      </c>
+      <c r="C7" s="23">
+        <f t="shared" si="0"/>
+        <v>7.4733317385149281E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <f>'DPP 2020'!J20</f>
+        <v>41550000</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>147218.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="3">
+        <v>28495000</v>
+      </c>
+      <c r="C8" s="23">
+        <f t="shared" si="0"/>
+        <v>7.2325226198763026E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <f>'DPP 2020'!J22</f>
+        <v>5250000</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>142475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="3">
+        <v>28450000</v>
+      </c>
+      <c r="C9" s="23">
+        <f t="shared" si="0"/>
+        <v>7.2211008434981849E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f>'DPP 2020'!J24</f>
+        <v>5500000</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>142250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="3">
+        <v>28275000</v>
+      </c>
+      <c r="C10" s="23">
+        <f t="shared" si="0"/>
+        <v>7.1766828242499539E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <f>'DPP 2020'!J27</f>
+        <v>12036364</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>141375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="3">
+        <v>29950000</v>
+      </c>
+      <c r="C11" s="23">
+        <f t="shared" si="0"/>
+        <v>7.6018267227687397E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7250000</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>149750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="3">
+        <v>26850000</v>
+      </c>
+      <c r="C12" s="23">
+        <f t="shared" si="0"/>
+        <v>6.8149932389429277E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <f>'DPP 2020'!J29</f>
+        <v>25500000</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>134250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42750000</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10850687559210806</v>
+      </c>
+      <c r="D13" s="3">
+        <f>'DPP 2020'!J33</f>
+        <v>155360909</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>213750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3">
+        <f>SUM(B2:B13)</f>
+        <v>393984250</v>
+      </c>
+      <c r="D15" s="3">
+        <f>SUM(D2:D13)</f>
+        <v>387877729</v>
+      </c>
+      <c r="F15" s="3">
+        <f>SUM(F2:F13)</f>
+        <v>1969921.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B15-B19</f>
+        <v>3271134.5500000119</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="F16" s="23">
+        <f>F15/B15</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="3">
+        <f>'DPP 2020'!G38</f>
+        <v>372107729</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="3">
+        <f>B18*1.05</f>
+        <v>390713115.44999999</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="3">
+        <f>B19/12</f>
+        <v>32559426.287499998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3313,7 +4066,7 @@
         <v>3054546</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H32" si="0">G4*0.1</f>
+        <f t="shared" ref="H4:H31" si="0">G4*0.1</f>
         <v>305454.60000000003</v>
       </c>
     </row>
@@ -4126,13 +4879,315 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3">
+        <v>41000000</v>
+      </c>
+      <c r="C2" s="23">
+        <f>B2/$B$15</f>
+        <v>0.31132895701002705</v>
+      </c>
+      <c r="D2" s="3">
+        <f>'DPP 2021'!J7</f>
+        <v>28634546</v>
+      </c>
+      <c r="F2" s="3">
+        <f>B2*0.005</f>
+        <v>205000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="3">
+        <v>32255500</v>
+      </c>
+      <c r="C3" s="23">
+        <f t="shared" ref="C3:C13" si="0">B3/$B$15</f>
+        <v>0.24492856519114459</v>
+      </c>
+      <c r="D3" s="3">
+        <f>'DPP 2021'!J11</f>
+        <v>13745455</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F13" si="1">B3*0.005</f>
+        <v>161277.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="3">
+        <v>26985000</v>
+      </c>
+      <c r="C4" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20490760743696537</v>
+      </c>
+      <c r="D4" s="3">
+        <f>'DPP 2021'!J14</f>
+        <v>82986818</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>134925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="3">
+        <v>31453000</v>
+      </c>
+      <c r="C5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23883487036186296</v>
+      </c>
+      <c r="D5" s="3">
+        <f>'DPP 2021'!J17</f>
+        <v>3345819</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>157265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3">
+        <f>SUM(B2:B13)</f>
+        <v>131693500</v>
+      </c>
+      <c r="D15" s="3">
+        <f>SUM(D2:D13)</f>
+        <v>128712638</v>
+      </c>
+      <c r="F15" s="3">
+        <f>SUM(F2:F13)</f>
+        <v>658467.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B15-D15</f>
+        <v>2980862</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="F16" s="23">
+        <f>F15/B15</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="3">
+        <f>B18*1.05</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="3">
+        <f>B19/12</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4651,7 +5706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -4696,7 +5751,7 @@
       </c>
       <c r="B3" s="4">
         <f>'DPP 2019'!G56</f>
-        <v>685649947</v>
+        <v>689413807</v>
       </c>
       <c r="C3" s="4">
         <f>'DPP 2019'!H56</f>

</xml_diff>